<commit_message>
fix change history sheet format and fix field name in json
</commit_message>
<xml_diff>
--- a/env/ccd-template.xlsx
+++ b/env/ccd-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdayican/projects/hmcts/bulk-scan-ccd-definitions/env/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240E660F-EFC9-7C44-A05D-B13F85C0D9E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB8689D-580C-F844-B472-BC2BD8EBB682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27660" windowHeight="13840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -691,10 +691,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="166" formatCode="d\ mmm\ yyyy"/>
   </numFmts>
   <fonts count="31" x14ac:knownFonts="1">
     <font>
@@ -954,7 +953,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1059,9 +1058,6 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1075,22 +1071,30 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1477,112 +1481,111 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
-    <col min="2" max="2" width="91.1640625" style="75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" style="84" customWidth="1"/>
+    <col min="2" max="2" width="91.1640625" style="74" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="29.5" customWidth="1"/>
+    <col min="4" max="4" width="29.5" style="81" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="77" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:5" s="76" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="82" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="75"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="78" t="s">
         <v>184</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="77" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="72" t="s">
+      <c r="D3" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="78" t="s">
+      <c r="E3" s="77" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C4" s="76"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="76"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="75"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C5" s="76"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="76"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="75"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C6" s="76"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="76"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="75"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C7" s="76"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="76"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="75"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C8" s="76"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="76"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="75"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="81"/>
-      <c r="B9" s="82"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="83"/>
+      <c r="A9" s="85"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="80"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D10" s="84"/>
-      <c r="E10" s="83"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="80"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D11" s="84"/>
-      <c r="E11" s="83"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="80"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D12" s="84"/>
-      <c r="E12" s="83"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="80"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D13" s="84"/>
-      <c r="E13" s="83"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="80"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D14" s="84"/>
-      <c r="E14" s="83"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="80"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D15" s="84"/>
-      <c r="E15" s="83"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="80"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D16" s="84"/>
-      <c r="E16" s="83"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="80"/>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D17" s="84"/>
-      <c r="E17" s="83"/>
+      <c r="D17" s="88"/>
+      <c r="E17" s="80"/>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D18" s="85"/>
-      <c r="E18" s="83"/>
+      <c r="E18" s="80"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix change history sheet format and fix field name in json (#37)
</commit_message>
<xml_diff>
--- a/env/ccd-template.xlsx
+++ b/env/ccd-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdayican/projects/hmcts/bulk-scan-ccd-definitions/env/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240E660F-EFC9-7C44-A05D-B13F85C0D9E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB8689D-580C-F844-B472-BC2BD8EBB682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27660" windowHeight="13840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -691,10 +691,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="166" formatCode="d\ mmm\ yyyy"/>
   </numFmts>
   <fonts count="31" x14ac:knownFonts="1">
     <font>
@@ -954,7 +953,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1059,9 +1058,6 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1075,22 +1071,30 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1477,112 +1481,111 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.1640625" customWidth="1"/>
-    <col min="2" max="2" width="91.1640625" style="75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" style="84" customWidth="1"/>
+    <col min="2" max="2" width="91.1640625" style="74" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" customWidth="1"/>
-    <col min="4" max="4" width="29.5" customWidth="1"/>
+    <col min="4" max="4" width="29.5" style="81" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="77" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:5" s="76" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="82" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="75"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="78" t="s">
+      <c r="A3" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="78" t="s">
         <v>184</v>
       </c>
-      <c r="C3" s="78" t="s">
+      <c r="C3" s="77" t="s">
         <v>185</v>
       </c>
-      <c r="D3" s="72" t="s">
+      <c r="D3" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="78" t="s">
+      <c r="E3" s="77" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C4" s="76"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="76"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="75"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C5" s="76"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="76"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="75"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C6" s="76"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="76"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="75"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C7" s="76"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="76"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="75"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C8" s="76"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="76"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="75"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="81"/>
-      <c r="B9" s="82"/>
-      <c r="C9" s="83"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="83"/>
+      <c r="A9" s="85"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="80"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D10" s="84"/>
-      <c r="E10" s="83"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="80"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D11" s="84"/>
-      <c r="E11" s="83"/>
+      <c r="D11" s="88"/>
+      <c r="E11" s="80"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D12" s="84"/>
-      <c r="E12" s="83"/>
+      <c r="D12" s="88"/>
+      <c r="E12" s="80"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D13" s="84"/>
-      <c r="E13" s="83"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="80"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D14" s="84"/>
-      <c r="E14" s="83"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="80"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D15" s="84"/>
-      <c r="E15" s="83"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="80"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D16" s="84"/>
-      <c r="E16" s="83"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="80"/>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D17" s="84"/>
-      <c r="E17" s="83"/>
+      <c r="D17" s="88"/>
+      <c r="E17" s="80"/>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D18" s="85"/>
-      <c r="E18" s="83"/>
+      <c r="E18" s="80"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>